<commit_message>
start jueu de la vie
</commit_message>
<xml_diff>
--- a/codingame_scraper/medium_20250202.xlsx
+++ b/codingame_scraper/medium_20250202.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/5102170ae7533958/Documents/Programmation/codingame_py/codingame_scraper/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="3" documentId="8_{E09026CA-BD3F-41B4-9345-23067BD1B31B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2CE803ED-B4B6-4893-98F0-7BABB9ADC5A8}"/>
+  <xr:revisionPtr revIDLastSave="4" documentId="8_{E09026CA-BD3F-41B4-9345-23067BD1B31B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{AC6A5FAE-4729-4605-BAEB-65753828E865}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="18696" xr2:uid="{1162784B-948C-44FC-AD72-3852461035BB}"/>
   </bookViews>
@@ -48,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="358" uniqueCount="335">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="359" uniqueCount="335">
   <si>
     <t>titre</t>
   </si>
@@ -1109,10 +1109,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1462,7 +1458,7 @@
   <dimension ref="A1:C333"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E26" sqref="E26"/>
+      <selection activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1730,6 +1726,9 @@
       </c>
       <c r="B24">
         <v>2364</v>
+      </c>
+      <c r="C24" t="s">
+        <v>332</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
custom game of life is done
</commit_message>
<xml_diff>
--- a/codingame_scraper/medium_20250202.xlsx
+++ b/codingame_scraper/medium_20250202.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/5102170ae7533958/Documents/Programmation/codingame_py/codingame_scraper/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="4" documentId="8_{E09026CA-BD3F-41B4-9345-23067BD1B31B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{AC6A5FAE-4729-4605-BAEB-65753828E865}"/>
+  <xr:revisionPtr revIDLastSave="6" documentId="8_{E09026CA-BD3F-41B4-9345-23067BD1B31B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{21C21B88-EE1C-42A3-94E6-E367CA904EB4}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="18696" xr2:uid="{1162784B-948C-44FC-AD72-3852461035BB}"/>
   </bookViews>
@@ -48,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="359" uniqueCount="335">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="361" uniqueCount="335">
   <si>
     <t>titre</t>
   </si>
@@ -1109,6 +1109,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1458,7 +1462,7 @@
   <dimension ref="A1:C333"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C24" sqref="C24"/>
+      <selection activeCell="C26" sqref="C26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1738,6 +1742,9 @@
       <c r="B25">
         <v>2261</v>
       </c>
+      <c r="C25" t="s">
+        <v>332</v>
+      </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
@@ -1745,6 +1752,9 @@
       </c>
       <c r="B26">
         <v>2155</v>
+      </c>
+      <c r="C26" t="s">
+        <v>332</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
start what_the_brainfuck prog language :-)
</commit_message>
<xml_diff>
--- a/codingame_scraper/medium_20250202.xlsx
+++ b/codingame_scraper/medium_20250202.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/5102170ae7533958/Documents/Programmation/codingame_py/codingame_scraper/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="6" documentId="8_{E09026CA-BD3F-41B4-9345-23067BD1B31B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{21C21B88-EE1C-42A3-94E6-E367CA904EB4}"/>
+  <xr:revisionPtr revIDLastSave="8" documentId="8_{E09026CA-BD3F-41B4-9345-23067BD1B31B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{94E4246A-CE64-4B98-9137-F289AB7406F0}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="18696" xr2:uid="{1162784B-948C-44FC-AD72-3852461035BB}"/>
   </bookViews>
@@ -48,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="361" uniqueCount="335">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="363" uniqueCount="335">
   <si>
     <t>titre</t>
   </si>
@@ -1462,7 +1462,7 @@
   <dimension ref="A1:C333"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C26" sqref="C26"/>
+      <selection activeCell="C28" sqref="C28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1764,6 +1764,9 @@
       <c r="B27">
         <v>1932</v>
       </c>
+      <c r="C27" t="s">
+        <v>332</v>
+      </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
@@ -1771,6 +1774,9 @@
       </c>
       <c r="B28">
         <v>1778</v>
+      </c>
+      <c r="C28" t="s">
+        <v>332</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
porcupine done. Start romans numbers
</commit_message>
<xml_diff>
--- a/codingame_scraper/medium_20250202.xlsx
+++ b/codingame_scraper/medium_20250202.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/5102170ae7533958/Documents/Programmation/codingame_py/codingame_scraper/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="8" documentId="8_{E09026CA-BD3F-41B4-9345-23067BD1B31B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{94E4246A-CE64-4B98-9137-F289AB7406F0}"/>
+  <xr:revisionPtr revIDLastSave="10" documentId="8_{E09026CA-BD3F-41B4-9345-23067BD1B31B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E834DB51-8DEB-4F3A-9763-AC6CA432F125}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="18696" xr2:uid="{1162784B-948C-44FC-AD72-3852461035BB}"/>
   </bookViews>
@@ -48,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="363" uniqueCount="335">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="365" uniqueCount="336">
   <si>
     <t>titre</t>
   </si>
@@ -1053,6 +1053,9 @@
   </si>
   <si>
     <t>There is no spoon</t>
+  </si>
+  <si>
+    <t>En cours</t>
   </si>
 </sst>
 </file>
@@ -1462,7 +1465,7 @@
   <dimension ref="A1:C333"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C28" sqref="C28"/>
+      <selection activeCell="G30" sqref="G30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1786,6 +1789,9 @@
       <c r="B29">
         <v>1748</v>
       </c>
+      <c r="C29" t="s">
+        <v>332</v>
+      </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
@@ -1793,6 +1799,9 @@
       </c>
       <c r="B30">
         <v>1712</v>
+      </c>
+      <c r="C30" t="s">
+        <v>335</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.3">

</xml_diff>